<commit_message>
Add media, migrate PCB work from Altium to Eagle. Creating new branch for PCB work
</commit_message>
<xml_diff>
--- a/BOMs/REV2-BOM.xlsx
+++ b/BOMs/REV2-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\AoM\IoT-Bit\AoM-IoT-Bit\PCB-shield\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\AoM\IoT-Bit\AoM-IoT-Bit\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B949DEFD-8D85-4663-A24A-64EFBF3D6506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FE5475-38F2-46FF-849B-5D469A94E299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:H28"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,7 +742,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H28" si="0">PRODUCT(E3*F3)</f>
+        <f t="shared" ref="H3:H20" si="0">PRODUCT(E3*F3)</f>
         <v>0.38</v>
       </c>
       <c r="I3" s="5" t="s">

</xml_diff>